<commit_message>
New updated default values
</commit_message>
<xml_diff>
--- a/VelocityRSD/VelocityRSD_model.xlsx
+++ b/VelocityRSD/VelocityRSD_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="7290" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10695" windowHeight="6885" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plot" sheetId="1" r:id="rId1"/>
@@ -424,11 +424,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353179896"/>
-        <c:axId val="353184208"/>
+        <c:axId val="388485696"/>
+        <c:axId val="388486480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353179896"/>
+        <c:axId val="388485696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,12 +484,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353184208"/>
+        <c:crossAx val="388486480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353184208"/>
+        <c:axId val="388486480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +546,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353179896"/>
+        <c:crossAx val="388485696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -883,11 +883,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353180680"/>
-        <c:axId val="353178328"/>
+        <c:axId val="388484128"/>
+        <c:axId val="388482560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353180680"/>
+        <c:axId val="388484128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,12 +943,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353178328"/>
+        <c:crossAx val="388482560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353178328"/>
+        <c:axId val="388482560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -1007,7 +1007,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353180680"/>
+        <c:crossAx val="388484128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -1176,19 +1176,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>88</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>48</c:v>
@@ -1200,22 +1200,22 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>61</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>63</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>65</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>48</c:v>
@@ -1224,142 +1224,142 @@
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>105</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>62</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>65</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>66</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>100</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>62</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>88</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>56</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="53">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="48">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53</c:v>
-                </c:pt>
                 <c:pt idx="54">
-                  <c:v>49</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>101</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1374,11 +1374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353183816"/>
-        <c:axId val="353181464"/>
+        <c:axId val="388480600"/>
+        <c:axId val="388482952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353183816"/>
+        <c:axId val="388480600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1434,12 +1434,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353181464"/>
+        <c:crossAx val="388482952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353181464"/>
+        <c:axId val="388482952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="140"/>
@@ -1498,7 +1498,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353183816"/>
+        <c:crossAx val="388480600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20"/>
@@ -1862,19 +1862,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>88</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>48</c:v>
@@ -1886,22 +1886,22 @@
                   <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>61</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>66</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>63</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>65</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>48</c:v>
@@ -1910,142 +1910,142 @@
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>90</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>105</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>62</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>65</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>66</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>100</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>62</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>88</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>56</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="40">
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>53</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>51</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>57</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>48</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="46">
                   <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="47">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="53">
                   <c:v>54</c:v>
                 </c:pt>
-                <c:pt idx="48">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>55</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>102</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>53</c:v>
-                </c:pt>
                 <c:pt idx="54">
-                  <c:v>49</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>59</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>101</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>52</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2060,11 +2060,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="353184600"/>
-        <c:axId val="353184992"/>
+        <c:axId val="393007128"/>
+        <c:axId val="393005168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="353184600"/>
+        <c:axId val="393007128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2121,12 +2121,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353184992"/>
+        <c:crossAx val="393005168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="353184992"/>
+        <c:axId val="393005168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2183,7 +2183,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="353184600"/>
+        <c:crossAx val="393007128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5772,8 +5772,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="E5" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5804,7 +5804,7 @@
       </c>
       <c r="C2">
         <f>ROUNDUP(((B2-$H$9)*($H$11-$H$12)/($H$10-$H$9)+$H$12),0)</f>
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
@@ -5840,7 +5840,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G4" t="s">
         <v>2</v>
@@ -5858,7 +5858,7 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G5" t="s">
         <v>3</v>
@@ -5876,7 +5876,7 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -5936,7 +5936,7 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
         <v>1</v>
@@ -5945,7 +5945,7 @@
         <v>37500</v>
       </c>
       <c r="I10">
-        <v>40000</v>
+        <v>37500</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -5978,13 +5978,13 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G12" t="s">
         <v>3</v>
       </c>
       <c r="H12">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="I12">
         <v>120</v>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -6011,7 +6011,7 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -6059,7 +6059,7 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -6095,7 +6095,7 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -6119,7 +6119,7 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -6143,7 +6143,7 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -6155,7 +6155,7 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -6167,7 +6167,7 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -6179,7 +6179,7 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -6191,7 +6191,7 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -6215,7 +6215,7 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -6227,7 +6227,7 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6239,7 +6239,7 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -6251,7 +6251,7 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -6275,7 +6275,7 @@
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -6287,7 +6287,7 @@
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -6299,7 +6299,7 @@
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -6311,7 +6311,7 @@
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6335,7 +6335,7 @@
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -6359,7 +6359,7 @@
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -6371,7 +6371,7 @@
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -6395,7 +6395,7 @@
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -6407,7 +6407,7 @@
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6431,7 +6431,7 @@
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -6443,7 +6443,7 @@
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -6455,7 +6455,7 @@
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -6467,7 +6467,7 @@
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -6479,7 +6479,7 @@
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -6491,7 +6491,7 @@
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -6515,7 +6515,7 @@
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -6539,7 +6539,7 @@
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -6551,7 +6551,7 @@
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -6575,7 +6575,7 @@
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -6587,7 +6587,7 @@
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -6599,7 +6599,7 @@
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>